<commit_message>
REPORTGEN-1240: update CWE 2025 Top25 compiance reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/CWE (2025) Top 25 Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/CWE (2025) Top 25 Full Detailed Report.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\CAST\ReportGenerator\1.30.0\Templates\Application\Top25 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramData\CAST\ReportGenerator\1.30.0\Templates\Application\Top25 2025 - passe 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE0C479-6A30-4553-B5EB-D2B6F6504782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA0B97A-8173-499A-A490-94117B8DEB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
-    <sheet name="CWE (2025) Top25" sheetId="9" r:id="rId2"/>
-    <sheet name="CWE (2025) Top25 details" sheetId="10" r:id="rId3"/>
+    <sheet name="Note" sheetId="11" r:id="rId2"/>
+    <sheet name="CWE (2025) Top25" sheetId="9" r:id="rId3"/>
+    <sheet name="CWE (2025) Top25 details" sheetId="10" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_Hlk217403028" localSheetId="1">Note!$C$2</definedName>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">Summary!#REF!</definedName>
     <definedName name="Application_Size" comment="TEXT;APPLICATION_SIZE_TYPE" localSheetId="0">Summary!$G$4</definedName>
     <definedName name="EmpVersion" comment="TEXT;EMP_VERSION" localSheetId="0">Summary!$E$1</definedName>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>Application Name:</t>
   </si>
@@ -153,6 +155,71 @@
   </si>
   <si>
     <t>2025 CWE Top 25 Most Dangerous Software Weaknesses Compliance details</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">CWE Mapping &amp; Data Propagation Logic
+Note on Data Evolution 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">To ensure maximum accuracy and coverage, we have implemented a propagation system for CWE-to-QR (Quality Rule) mapping.
+Because the MITRE Top 25 includes high-level abstractions CWE ID (specifically a Pillar), we designed this mechanism to aggregate data from all descendant levels. This ensures that sections associated with a high-level category—which could have been previously empty—now accurately reflect the cumulative violations of quality rules decorated with descendant CWE IDs.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The Hierarchy &amp; Impact</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>•	Populated High-Level Views: Data now flows logically upward through all five abstraction levels of the CWE hierarchy:
+                        Variant → Base → Class → Category → Pillar  
+•	Comprehensive Reporting: Sections associated with Pillars, Categories, or Classes are now fully populated with the violations of their respective Base and Variant descendants.
+•	Mapping Best Practices: While the report aggregates data at the top three levels for visibility, Quality Rules remain mapped at the Base or Variant levels to maintain technical precision, as recommended by MITRE.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -162,7 +229,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +303,30 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -359,7 +450,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -445,6 +536,36 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -522,6 +643,61 @@
         <a:xfrm>
           <a:off x="10122477" y="207818"/>
           <a:ext cx="959387" cy="360000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>213013</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>69619</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1203573</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66630</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10D78363-93BA-460C-84B8-75BC000D9A53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10675273" y="260119"/>
+          <a:ext cx="990560" cy="492311"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -823,7 +999,7 @@
   <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,6 +1149,208 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5CEE97-BC24-4924-92B2-A711BE38CADB}">
+  <dimension ref="B1:G21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="2" max="2" width="75.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" customWidth="1"/>
+    <col min="13" max="13" width="36.5546875" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="3"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="2:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="35"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="38"/>
+    </row>
+    <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="38"/>
+    </row>
+    <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="38"/>
+    </row>
+    <row r="6" spans="2:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="38"/>
+    </row>
+    <row r="7" spans="2:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="38"/>
+    </row>
+    <row r="8" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
+    </row>
+    <row r="9" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="38"/>
+    </row>
+    <row r="10" spans="2:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="38"/>
+    </row>
+    <row r="11" spans="2:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="38"/>
+    </row>
+    <row r="12" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
+    </row>
+    <row r="13" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="36"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="38"/>
+    </row>
+    <row r="14" spans="2:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="36"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="38"/>
+    </row>
+    <row r="15" spans="2:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="36"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+    </row>
+    <row r="16" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="36"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+    </row>
+    <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="36"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="38"/>
+    </row>
+    <row r="18" spans="2:7" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="38"/>
+    </row>
+    <row r="19" spans="2:7" ht="15.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="38"/>
+    </row>
+    <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="38"/>
+    </row>
+    <row r="21" spans="2:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="39"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B2:G21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -1031,7 +1409,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00038B0F-4F74-4ACF-8A7F-FE15A067CF76}">
   <dimension ref="A1:H2"/>
   <sheetViews>

</xml_diff>